<commit_message>
choviwu api is finish and also add cache to develop performance
</commit_message>
<xml_diff>
--- a/design/database/gc-createTable.xlsx
+++ b/design/database/gc-createTable.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="92">
   <si>
     <t>序号</t>
   </si>
@@ -296,6 +296,78 @@
   </si>
   <si>
     <t>表编码:  T_GC_BU_GARBAGE_CLASSIFICATION</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表名称:  值列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注说明:  值列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>值列ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型编码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型包含值编码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型包含值的映射值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>顺序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>否</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LKV_ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOOKUP_TYPE_CODE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOOKUP_TYPE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOOKUP_VALUE_CODE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOOKUP_VALUE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ORDER_NO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表编码:  T_GC_DB_LOOKUP_VALUE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -668,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:L55"/>
+  <dimension ref="B3:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1384,7 +1456,7 @@
     </row>
     <row r="33" spans="3:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C33" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>32</v>
@@ -1410,7 +1482,7 @@
     </row>
     <row r="34" spans="3:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C34" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>39</v>
@@ -1438,7 +1510,7 @@
     </row>
     <row r="35" spans="3:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C35" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>35</v>
@@ -1466,7 +1538,7 @@
     </row>
     <row r="36" spans="3:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C36" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>41</v>
@@ -1504,27 +1576,305 @@
     </row>
     <row r="38" spans="3:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
+      <c r="D38" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
+      <c r="F38" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
+      <c r="J38" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-    </row>
-    <row r="55" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
-      <c r="K55" s="2"/>
+      <c r="L38" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="3:12" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C39" s="2"/>
+      <c r="D39" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="3:12" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C40" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L40" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="3:12" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C41" s="1">
+        <v>1</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="3:12" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C42" s="1">
+        <v>2</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G42" s="1">
+        <v>50</v>
+      </c>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="3:12" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C43" s="1">
+        <v>3</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G43" s="1">
+        <v>50</v>
+      </c>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="3:12" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C44" s="1">
+        <v>4</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G44" s="1">
+        <v>50</v>
+      </c>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="3:12" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C45" s="1">
+        <v>5</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G45" s="1">
+        <v>50</v>
+      </c>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="3:12" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C46" s="1">
+        <v>6</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="3:12" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C47" s="1">
+        <v>7</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="3:12" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C48" s="1">
+        <v>8</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>